<commit_message>
Add and modify some files.
</commit_message>
<xml_diff>
--- a/Leetcode Problems Statistic 20220325/Sorted_Problems.xlsx
+++ b/Leetcode Problems Statistic 20220325/Sorted_Problems.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\Leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\Leetcode\Leetcode Problems Statistic 20220325\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913D2EFC-F192-47CE-856F-F53F81F5E771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1D7C0D-DD4D-495E-830B-4BE2CBB71415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17896,7 +17896,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BX2570"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>